<commit_message>
Modificaciones finales a los vectores de prueba
</commit_message>
<xml_diff>
--- a/Proyecto1/timesSHA.xlsx
+++ b/Proyecto1/timesSHA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AbrilVzqz/Documents/Facultad de Ingeniería/10Semestre/Criptografía/Proyecto1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{94C89C4F-B60E-194E-9352-2FFEE13505EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A24ADA-BD99-404E-B233-0711191727F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="21880" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="timesSHA" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">timesSHA!$B$3:$B$18</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">timesSHA!$C$3:$C$18</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">timesSHA!$D$3:$D$18</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>SHA-1</t>
   </si>
@@ -33,11 +38,17 @@
   <si>
     <t>Tiempos Hashing</t>
   </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="12"/>
@@ -368,7 +379,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFEEE0AC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,18 +549,16 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -597,6 +606,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEEE0AC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -606,6 +620,1272 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl"/>
+              <a:t>Tiempos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES_tradnl" baseline="0"/>
+              <a:t> Funciones Has</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SHA-1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>timesSHA!$A$3:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Promedio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>timesSHA!$B$3:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>4.0000000000005302E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.10000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1000000000003999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0000000000002999E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0000000000002999E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3000000000006E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2000000000004999E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0000000000002999E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.19999999999981E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.1000000000004598E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.29999999999991E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.40000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3000000000006E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.10000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3000000000002101E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.0266666666669296E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3C1D-7143-A619-381CCA2C61CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>SHA-2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>timesSHA!$A$3:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Promedio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>timesSHA!$C$3:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2.5999999999998199E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.40000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0999999999997099E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9999999999961197E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9000000000000398E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2000000000004999E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0999999999997099E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0999999999997099E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.40000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.60000000000021E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.40000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.40000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.49999999999941E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9999999999995301E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.6000000000005101E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8199999999999199E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3C1D-7143-A619-381CCA2C61CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>SHA-3</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>timesSHA!$A$3:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Promedio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>timesSHA!$D$3:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1.98000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.40000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2000000000004999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1000000000003999E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0999999999997099E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.19999999999981E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0000000000002999E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0999999999997099E-5</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>1.1699999999999899E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.60000000000021E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.79999999999971E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.80000000000041E-5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.79999999999971E-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8999999999997302E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.8999999999997302E-5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.6266666666666758E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3C1D-7143-A619-381CCA2C61CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="359144975"/>
+        <c:axId val="370228479"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="359144975"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="370228479"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="370228479"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359144975"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDCE8848-4267-DF43-8F1C-96BFF11A5412}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -904,172 +2184,271 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2">
-        <v>3.0999999999996302E-5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.89999999999981E-5</v>
-      </c>
-      <c r="C3" s="2">
+    <row r="3" spans="1:4">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
         <v>4.0000000000005302E-5</v>
       </c>
+      <c r="C3" s="5">
+        <v>2.5999999999998199E-5</v>
+      </c>
+      <c r="D3">
+        <v>1.98000000000003E-4</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2">
-        <v>7.1000000000001604E-5</v>
-      </c>
-      <c r="B4" s="2">
+    <row r="4" spans="1:4">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2.10000000000001E-5</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.40000000000001E-5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1.40000000000001E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1.1000000000003999E-5</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1.0999999999997099E-5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1.2000000000004999E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
         <v>1.0000000000002999E-5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C6" s="5">
+        <v>9.9999999999961197E-6</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1.1000000000003999E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1.0000000000002999E-5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4.9000000000000398E-5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.0999999999997099E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.3000000000006E-5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.2000000000004999E-5</v>
+      </c>
+      <c r="D8" s="5">
         <v>1.19999999999981E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2">
+    <row r="9" spans="1:4">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1.2000000000004999E-5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1.0999999999997099E-5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.0000000000002999E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1.0000000000002999E-5</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.0999999999997099E-5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.0999999999997099E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1.19999999999981E-5</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1.40000000000001E-5</v>
+      </c>
+      <c r="D11">
+        <v>1.1699999999999899E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>8.1000000000004598E-5</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1.60000000000021E-5</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.60000000000021E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
         <v>1.29999999999991E-5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C13" s="5">
+        <v>1.40000000000001E-5</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1.79999999999971E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1.40000000000001E-5</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.40000000000001E-5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1.80000000000041E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1.3000000000006E-5</v>
+      </c>
+      <c r="C15" s="5">
         <v>1.49999999999941E-5</v>
       </c>
-      <c r="C5" s="2">
-        <v>1.0999999999997099E-5</v>
+      <c r="D15" s="5">
+        <v>1.79999999999971E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2">
-        <v>1.29999999999991E-5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1.0999999999997099E-5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>9.0000000000020602E-6</v>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2.10000000000001E-5</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2.9999999999995301E-5</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3.8999999999997302E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2">
-        <v>9.9999999999961197E-6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>7.00000000000006E-6</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.0000000000002999E-5</v>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2.3000000000002101E-5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2.6000000000005101E-5</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3.8999999999997302E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2">
-        <v>1.0000000000002999E-5</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2.10000000000001E-5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>5.9999999999990599E-6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2">
-        <v>1.0999999999997099E-5</v>
-      </c>
-      <c r="B9" s="2">
-        <v>7.9999999999941195E-6</v>
-      </c>
-      <c r="C9" s="2">
-        <v>7.00000000000006E-6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2">
-        <v>2.8000000000000199E-5</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1.1000000000003999E-5</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1.60000000000021E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>2.5999999999998199E-5</v>
-      </c>
-      <c r="B11" s="2">
-        <v>8.0000000000010601E-6</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1.15000000000003E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2">
-        <v>1.0000000000002999E-5</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1.60000000000021E-5</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1.60000000000021E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
-        <v>1.29999999999991E-5</v>
-      </c>
-      <c r="B13" s="2">
-        <v>3.2999999999998302E-5</v>
-      </c>
-      <c r="C13" s="2">
-        <v>4.9999999999994398E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4">
-        <f>AVERAGE(A3:A13)</f>
-        <v>2.1454545454544801E-5</v>
-      </c>
-      <c r="B14" s="4">
-        <f t="shared" ref="B14:C14" si="0">AVERAGE(B3:B13)</f>
-        <v>1.4454545454544732E-5</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" si="0"/>
-        <v>2.6545454545455116E-5</v>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5">
+        <f>AVERAGE(B3:B17)</f>
+        <v>2.0266666666669296E-5</v>
+      </c>
+      <c r="C18" s="5">
+        <f>AVERAGE(C3:C17)</f>
+        <v>1.8199999999999199E-5</v>
+      </c>
+      <c r="D18" s="5">
+        <f>AVERAGE(D3:D17)</f>
+        <v>3.6266666666666758E-5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>